<commit_message>
first pdf made with correct spacing
</commit_message>
<xml_diff>
--- a/ventiellijst 2345.xlsx
+++ b/ventiellijst 2345.xlsx
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="11">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -1014,7 +1014,7 @@
         <v>51</v>
       </c>
       <c r="L2" s="11">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="16">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -1042,7 +1042,7 @@
         <v>52</v>
       </c>
       <c r="L3" s="16">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -1057,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="16">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1070,7 +1070,7 @@
         <v>53</v>
       </c>
       <c r="L4" s="16">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
@@ -1098,7 +1098,7 @@
         <v>54</v>
       </c>
       <c r="L5" s="16">
-        <v>70</v>
+        <v>99</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -1126,7 +1126,7 @@
         <v>55</v>
       </c>
       <c r="L6" s="16">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
@@ -1154,7 +1154,7 @@
         <v>56</v>
       </c>
       <c r="L7" s="16">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -1182,7 +1182,7 @@
         <v>57</v>
       </c>
       <c r="L8" s="16">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
@@ -1210,7 +1210,7 @@
         <v>58</v>
       </c>
       <c r="L9" s="19">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="M9" s="20"/>
       <c r="N9" s="20"/>
@@ -1225,7 +1225,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="16">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
@@ -1238,7 +1238,7 @@
         <v>59</v>
       </c>
       <c r="L10" s="16">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
@@ -1253,7 +1253,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="24">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -1266,7 +1266,7 @@
         <v>60</v>
       </c>
       <c r="L11" s="24">
-        <v>70</v>
+        <v>94</v>
       </c>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
@@ -1298,7 +1298,7 @@
         <v>61</v>
       </c>
       <c r="L12" s="11">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -1313,7 +1313,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="16">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -1341,7 +1341,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="16">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
@@ -1354,7 +1354,7 @@
         <v>63</v>
       </c>
       <c r="L14" s="16">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -1369,7 +1369,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="16">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -1382,7 +1382,7 @@
         <v>64</v>
       </c>
       <c r="L15" s="16">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
@@ -1410,7 +1410,7 @@
         <v>65</v>
       </c>
       <c r="L16" s="16">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
@@ -1438,7 +1438,7 @@
         <v>66</v>
       </c>
       <c r="L17" s="16">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
@@ -1453,7 +1453,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="16">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
@@ -1466,7 +1466,7 @@
         <v>67</v>
       </c>
       <c r="L18" s="16">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
@@ -1494,7 +1494,7 @@
         <v>68</v>
       </c>
       <c r="L19" s="19">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M19" s="20"/>
       <c r="N19" s="20"/>
@@ -1522,7 +1522,7 @@
         <v>69</v>
       </c>
       <c r="L20" s="16">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
@@ -1567,7 +1567,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="11">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
@@ -1582,7 +1582,7 @@
         <v>71</v>
       </c>
       <c r="L22" s="11">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
@@ -1597,7 +1597,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="16">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -1610,7 +1610,7 @@
         <v>72</v>
       </c>
       <c r="L23" s="16">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -1625,7 +1625,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="16">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -1638,7 +1638,7 @@
         <v>73</v>
       </c>
       <c r="L24" s="16">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -1653,7 +1653,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="16">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="17"/>
@@ -1666,7 +1666,7 @@
         <v>74</v>
       </c>
       <c r="L25" s="16">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
@@ -1694,7 +1694,7 @@
         <v>75</v>
       </c>
       <c r="L26" s="16">
-        <v>92</v>
+        <v>61</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
@@ -1709,7 +1709,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="16">
-        <v>104</v>
+        <v>112</v>
       </c>
       <c r="D27" s="17"/>
       <c r="E27" s="17"/>
@@ -1722,7 +1722,7 @@
         <v>76</v>
       </c>
       <c r="L27" s="16">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
@@ -1737,7 +1737,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="16">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
@@ -1750,7 +1750,7 @@
         <v>77</v>
       </c>
       <c r="L28" s="16">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
@@ -1765,7 +1765,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="19">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
@@ -1778,7 +1778,7 @@
         <v>78</v>
       </c>
       <c r="L29" s="19">
-        <v>89</v>
+        <v>46</v>
       </c>
       <c r="M29" s="20"/>
       <c r="N29" s="20"/>
@@ -1793,7 +1793,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="16">
-        <v>8</v>
+        <v>106</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -1806,7 +1806,7 @@
         <v>79</v>
       </c>
       <c r="L30" s="16">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -1821,7 +1821,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="24">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
@@ -1834,7 +1834,7 @@
         <v>80</v>
       </c>
       <c r="L31" s="24">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="M31" s="25"/>
       <c r="N31" s="25"/>
@@ -1851,7 +1851,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="11">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -1866,7 +1866,7 @@
         <v>81</v>
       </c>
       <c r="L32" s="11">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
@@ -1881,7 +1881,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="16">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -1894,7 +1894,7 @@
         <v>82</v>
       </c>
       <c r="L33" s="16">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
@@ -1909,7 +1909,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="16">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -1922,7 +1922,7 @@
         <v>83</v>
       </c>
       <c r="L34" s="16">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -1937,7 +1937,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="16">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -1950,7 +1950,7 @@
         <v>84</v>
       </c>
       <c r="L35" s="16">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -1965,7 +1965,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="16">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -1978,7 +1978,7 @@
         <v>85</v>
       </c>
       <c r="L36" s="16">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -1993,7 +1993,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="16">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
@@ -2006,7 +2006,7 @@
         <v>86</v>
       </c>
       <c r="L37" s="16">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
@@ -2021,7 +2021,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="16">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -2034,7 +2034,7 @@
         <v>87</v>
       </c>
       <c r="L38" s="16">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
@@ -2049,7 +2049,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="19">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D39" s="20"/>
       <c r="E39" s="20"/>
@@ -2062,7 +2062,7 @@
         <v>88</v>
       </c>
       <c r="L39" s="19">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M39" s="20"/>
       <c r="N39" s="20"/>
@@ -2077,7 +2077,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="16">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="D40" s="17"/>
       <c r="E40" s="17"/>
@@ -2090,7 +2090,7 @@
         <v>89</v>
       </c>
       <c r="L40" s="16">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
@@ -2105,7 +2105,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="24">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="D41" s="25"/>
       <c r="E41" s="25"/>
@@ -2118,7 +2118,7 @@
         <v>90</v>
       </c>
       <c r="L41" s="24">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M41" s="25"/>
       <c r="N41" s="25"/>
@@ -2135,7 +2135,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="11">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -2150,7 +2150,7 @@
         <v>91</v>
       </c>
       <c r="L42" s="11">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
@@ -2165,7 +2165,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="16">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
@@ -2178,7 +2178,7 @@
         <v>92</v>
       </c>
       <c r="L43" s="16">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
@@ -2193,7 +2193,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="16">
-        <v>81</v>
+        <v>107</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
@@ -2206,7 +2206,7 @@
         <v>93</v>
       </c>
       <c r="L44" s="16">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
@@ -2221,7 +2221,7 @@
         <v>44</v>
       </c>
       <c r="C45" s="16">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
@@ -2234,7 +2234,7 @@
         <v>94</v>
       </c>
       <c r="L45" s="16">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
@@ -2249,7 +2249,7 @@
         <v>45</v>
       </c>
       <c r="C46" s="16">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -2262,7 +2262,7 @@
         <v>95</v>
       </c>
       <c r="L46" s="16">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
@@ -2277,7 +2277,7 @@
         <v>46</v>
       </c>
       <c r="C47" s="16">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -2290,7 +2290,7 @@
         <v>96</v>
       </c>
       <c r="L47" s="16">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -2305,7 +2305,7 @@
         <v>47</v>
       </c>
       <c r="C48" s="16">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -2318,7 +2318,7 @@
         <v>97</v>
       </c>
       <c r="L48" s="16">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
@@ -2333,7 +2333,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="19">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D49" s="20"/>
       <c r="E49" s="20"/>
@@ -2346,7 +2346,7 @@
         <v>98</v>
       </c>
       <c r="L49" s="19">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M49" s="20"/>
       <c r="N49" s="20"/>
@@ -2361,7 +2361,7 @@
         <v>49</v>
       </c>
       <c r="C50" s="16">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
@@ -2374,7 +2374,7 @@
         <v>99</v>
       </c>
       <c r="L50" s="16">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -2389,7 +2389,7 @@
         <v>50</v>
       </c>
       <c r="C51" s="24">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="25"/>
@@ -2402,7 +2402,7 @@
         <v>100</v>
       </c>
       <c r="L51" s="24">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="M51" s="25"/>
       <c r="N51" s="25"/>
@@ -2467,7 +2467,7 @@
         <v>101</v>
       </c>
       <c r="C53" s="11">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="D53" s="12"/>
       <c r="E53" s="12"/>
@@ -2482,7 +2482,7 @@
         <v>151</v>
       </c>
       <c r="L53" s="11">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="M53" s="12"/>
       <c r="N53" s="12"/>
@@ -2497,7 +2497,7 @@
         <v>102</v>
       </c>
       <c r="C54" s="16">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D54" s="17"/>
       <c r="E54" s="17"/>
@@ -2510,7 +2510,7 @@
         <v>152</v>
       </c>
       <c r="L54" s="16">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="M54" s="17"/>
       <c r="N54" s="17"/>
@@ -2525,7 +2525,7 @@
         <v>103</v>
       </c>
       <c r="C55" s="16">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D55" s="17"/>
       <c r="E55" s="17"/>
@@ -2538,7 +2538,7 @@
         <v>153</v>
       </c>
       <c r="L55" s="16">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
@@ -2553,7 +2553,7 @@
         <v>104</v>
       </c>
       <c r="C56" s="16">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D56" s="17"/>
       <c r="E56" s="17"/>
@@ -2566,7 +2566,7 @@
         <v>154</v>
       </c>
       <c r="L56" s="16">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M56" s="17"/>
       <c r="N56" s="17"/>
@@ -2581,7 +2581,7 @@
         <v>105</v>
       </c>
       <c r="C57" s="16">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
@@ -2594,7 +2594,7 @@
         <v>155</v>
       </c>
       <c r="L57" s="16">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
@@ -2609,7 +2609,7 @@
         <v>106</v>
       </c>
       <c r="C58" s="16">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
@@ -2622,7 +2622,7 @@
         <v>156</v>
       </c>
       <c r="L58" s="16">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="M58" s="17"/>
       <c r="N58" s="17"/>
@@ -2637,7 +2637,7 @@
         <v>107</v>
       </c>
       <c r="C59" s="16">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
@@ -2650,7 +2650,7 @@
         <v>157</v>
       </c>
       <c r="L59" s="16">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="M59" s="17"/>
       <c r="N59" s="17"/>
@@ -2665,7 +2665,7 @@
         <v>108</v>
       </c>
       <c r="C60" s="19">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
@@ -2678,7 +2678,7 @@
         <v>158</v>
       </c>
       <c r="L60" s="19">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="M60" s="20"/>
       <c r="N60" s="20"/>
@@ -2693,7 +2693,7 @@
         <v>109</v>
       </c>
       <c r="C61" s="16">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D61" s="17"/>
       <c r="E61" s="17"/>
@@ -2706,7 +2706,7 @@
         <v>159</v>
       </c>
       <c r="L61" s="16">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="M61" s="17"/>
       <c r="N61" s="17"/>
@@ -2734,7 +2734,7 @@
         <v>160</v>
       </c>
       <c r="L62" s="24">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="M62" s="25"/>
       <c r="N62" s="25"/>
@@ -2751,7 +2751,7 @@
         <v>111</v>
       </c>
       <c r="C63" s="11">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -2781,7 +2781,7 @@
         <v>112</v>
       </c>
       <c r="C64" s="16">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D64" s="17"/>
       <c r="E64" s="17"/>
@@ -2809,7 +2809,7 @@
         <v>113</v>
       </c>
       <c r="C65" s="16">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D65" s="17"/>
       <c r="E65" s="17"/>
@@ -2865,7 +2865,7 @@
         <v>115</v>
       </c>
       <c r="C67" s="16">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D67" s="17"/>
       <c r="E67" s="17"/>
@@ -2893,7 +2893,7 @@
         <v>116</v>
       </c>
       <c r="C68" s="16">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D68" s="17"/>
       <c r="E68" s="17"/>
@@ -2921,7 +2921,7 @@
         <v>117</v>
       </c>
       <c r="C69" s="16">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D69" s="17"/>
       <c r="E69" s="17"/>
@@ -2949,7 +2949,7 @@
         <v>118</v>
       </c>
       <c r="C70" s="19">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D70" s="20"/>
       <c r="E70" s="20"/>
@@ -2977,7 +2977,7 @@
         <v>119</v>
       </c>
       <c r="C71" s="16">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D71" s="17"/>
       <c r="E71" s="17"/>
@@ -2990,7 +2990,7 @@
         <v>169</v>
       </c>
       <c r="L71" s="16">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="M71" s="17"/>
       <c r="N71" s="17"/>
@@ -3005,7 +3005,7 @@
         <v>120</v>
       </c>
       <c r="C72" s="24">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D72" s="25"/>
       <c r="E72" s="25"/>
@@ -3018,7 +3018,7 @@
         <v>170</v>
       </c>
       <c r="L72" s="24">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M72" s="25"/>
       <c r="N72" s="25"/>
@@ -3035,7 +3035,7 @@
         <v>121</v>
       </c>
       <c r="C73" s="11">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -3065,7 +3065,7 @@
         <v>122</v>
       </c>
       <c r="C74" s="16">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
@@ -3093,7 +3093,7 @@
         <v>123</v>
       </c>
       <c r="C75" s="16">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="D75" s="17"/>
       <c r="E75" s="17"/>
@@ -3121,7 +3121,7 @@
         <v>124</v>
       </c>
       <c r="C76" s="16">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D76" s="17"/>
       <c r="E76" s="17"/>
@@ -3149,7 +3149,7 @@
         <v>125</v>
       </c>
       <c r="C77" s="16">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D77" s="17"/>
       <c r="E77" s="17"/>
@@ -3177,7 +3177,7 @@
         <v>126</v>
       </c>
       <c r="C78" s="16">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D78" s="17"/>
       <c r="E78" s="17"/>
@@ -3190,7 +3190,7 @@
         <v>176</v>
       </c>
       <c r="L78" s="16">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M78" s="17"/>
       <c r="N78" s="17"/>
@@ -3205,7 +3205,7 @@
         <v>127</v>
       </c>
       <c r="C79" s="16">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D79" s="17"/>
       <c r="E79" s="17"/>
@@ -3261,7 +3261,7 @@
         <v>129</v>
       </c>
       <c r="C81" s="16">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D81" s="17"/>
       <c r="E81" s="17"/>
@@ -3289,7 +3289,7 @@
         <v>130</v>
       </c>
       <c r="C82" s="24">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D82" s="25"/>
       <c r="E82" s="25"/>
@@ -3319,7 +3319,7 @@
         <v>131</v>
       </c>
       <c r="C83" s="11">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
@@ -3349,7 +3349,7 @@
         <v>132</v>
       </c>
       <c r="C84" s="16">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D84" s="17"/>
       <c r="E84" s="17"/>
@@ -3377,7 +3377,7 @@
         <v>133</v>
       </c>
       <c r="C85" s="16">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D85" s="17"/>
       <c r="E85" s="17"/>
@@ -3405,7 +3405,7 @@
         <v>134</v>
       </c>
       <c r="C86" s="16">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D86" s="17"/>
       <c r="E86" s="17"/>
@@ -3418,7 +3418,7 @@
         <v>184</v>
       </c>
       <c r="L86" s="16">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="M86" s="17"/>
       <c r="N86" s="17"/>
@@ -3433,7 +3433,7 @@
         <v>135</v>
       </c>
       <c r="C87" s="16">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D87" s="17"/>
       <c r="E87" s="17"/>
@@ -3446,7 +3446,7 @@
         <v>185</v>
       </c>
       <c r="L87" s="16">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="M87" s="17"/>
       <c r="N87" s="17"/>
@@ -3461,7 +3461,7 @@
         <v>136</v>
       </c>
       <c r="C88" s="16">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D88" s="17"/>
       <c r="E88" s="17"/>
@@ -3489,7 +3489,7 @@
         <v>137</v>
       </c>
       <c r="C89" s="16">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D89" s="17"/>
       <c r="E89" s="17"/>
@@ -3517,7 +3517,7 @@
         <v>138</v>
       </c>
       <c r="C90" s="19">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="D90" s="20"/>
       <c r="E90" s="20"/>
@@ -3530,7 +3530,7 @@
         <v>188</v>
       </c>
       <c r="L90" s="19">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M90" s="20"/>
       <c r="N90" s="20"/>
@@ -3558,7 +3558,7 @@
         <v>189</v>
       </c>
       <c r="L91" s="16">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M91" s="17"/>
       <c r="N91" s="17"/>
@@ -3573,7 +3573,7 @@
         <v>140</v>
       </c>
       <c r="C92" s="24">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D92" s="25"/>
       <c r="E92" s="25"/>
@@ -3586,7 +3586,7 @@
         <v>190</v>
       </c>
       <c r="L92" s="24">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="M92" s="25"/>
       <c r="N92" s="25"/>
@@ -3603,7 +3603,7 @@
         <v>141</v>
       </c>
       <c r="C93" s="11">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
@@ -3618,7 +3618,7 @@
         <v>142</v>
       </c>
       <c r="C94" s="16">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D94" s="17"/>
       <c r="E94" s="17"/>
@@ -3633,7 +3633,7 @@
         <v>143</v>
       </c>
       <c r="C95" s="16">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D95" s="17"/>
       <c r="E95" s="17"/>
@@ -3648,7 +3648,7 @@
         <v>144</v>
       </c>
       <c r="C96" s="16">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D96" s="17"/>
       <c r="E96" s="17"/>
@@ -3663,7 +3663,7 @@
         <v>145</v>
       </c>
       <c r="C97" s="16">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D97" s="17"/>
       <c r="E97" s="17"/>
@@ -3678,7 +3678,7 @@
         <v>146</v>
       </c>
       <c r="C98" s="16">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D98" s="17"/>
       <c r="E98" s="17"/>
@@ -3693,7 +3693,7 @@
         <v>147</v>
       </c>
       <c r="C99" s="16">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D99" s="17"/>
       <c r="E99" s="17"/>
@@ -3708,7 +3708,7 @@
         <v>148</v>
       </c>
       <c r="C100" s="19">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D100" s="20"/>
       <c r="E100" s="20"/>
@@ -3723,7 +3723,7 @@
         <v>149</v>
       </c>
       <c r="C101" s="16">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
@@ -3738,7 +3738,7 @@
         <v>150</v>
       </c>
       <c r="C102" s="24">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D102" s="25"/>
       <c r="E102" s="25"/>
@@ -3841,7 +3841,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="28">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -3856,7 +3856,7 @@
         <v>25</v>
       </c>
       <c r="L2" s="28">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -3871,7 +3871,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="29">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -3884,7 +3884,7 @@
         <v>26</v>
       </c>
       <c r="L3" s="29">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -3899,7 +3899,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="29">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -3912,7 +3912,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="29">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
@@ -3927,7 +3927,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="29">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -3940,7 +3940,7 @@
         <v>28</v>
       </c>
       <c r="L5" s="29">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
@@ -3957,7 +3957,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="28">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -3987,7 +3987,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="29">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -4015,7 +4015,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="29">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -4043,7 +4043,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="29">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -4073,7 +4073,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="28">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -4103,7 +4103,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="29">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -4131,7 +4131,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="29">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -4159,7 +4159,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="29">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
@@ -4172,7 +4172,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="29">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
@@ -4189,7 +4189,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="28">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -4219,7 +4219,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="29">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -4247,7 +4247,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="29">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -4275,7 +4275,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="29">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -4320,7 +4320,7 @@
         <v>41</v>
       </c>
       <c r="L18" s="28">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
@@ -4335,7 +4335,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="29">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D19" s="17"/>
       <c r="E19" s="17"/>
@@ -4348,7 +4348,7 @@
         <v>42</v>
       </c>
       <c r="L19" s="29">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
@@ -4376,7 +4376,7 @@
         <v>43</v>
       </c>
       <c r="L20" s="29">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
@@ -4391,7 +4391,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="31">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
@@ -4404,7 +4404,7 @@
         <v>44</v>
       </c>
       <c r="L21" s="29">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
@@ -4436,7 +4436,7 @@
         <v>45</v>
       </c>
       <c r="L22" s="28">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
@@ -4451,7 +4451,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="29">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -4464,7 +4464,7 @@
         <v>46</v>
       </c>
       <c r="L23" s="29">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -4479,7 +4479,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="29">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -4492,7 +4492,7 @@
         <v>47</v>
       </c>
       <c r="L24" s="29">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -4599,7 +4599,7 @@
         <v>1</v>
       </c>
       <c r="C29" s="40">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
@@ -4629,7 +4629,7 @@
         <v>2</v>
       </c>
       <c r="C30" s="29">
-        <v>112</v>
+        <v>10</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -4642,7 +4642,7 @@
         <v>32</v>
       </c>
       <c r="L30" s="29">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -4681,7 +4681,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="29">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
@@ -4709,7 +4709,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="29">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -4739,7 +4739,7 @@
         <v>6</v>
       </c>
       <c r="C34" s="28">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="D34" s="12"/>
       <c r="E34" s="12"/>
@@ -4754,7 +4754,7 @@
         <v>36</v>
       </c>
       <c r="L34" s="28">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
@@ -4769,7 +4769,7 @@
         <v>7</v>
       </c>
       <c r="C35" s="29">
-        <v>108</v>
+        <v>10</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -4782,7 +4782,7 @@
         <v>37</v>
       </c>
       <c r="L35" s="29">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -4821,7 +4821,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="29">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17"/>
@@ -4849,7 +4849,7 @@
         <v>10</v>
       </c>
       <c r="C38" s="29">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -4879,7 +4879,7 @@
         <v>11</v>
       </c>
       <c r="C39" s="28">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="D39" s="12"/>
       <c r="E39" s="12"/>
@@ -4909,7 +4909,7 @@
         <v>12</v>
       </c>
       <c r="C40" s="40">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
@@ -4922,7 +4922,7 @@
         <v>42</v>
       </c>
       <c r="L40" s="40">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M40" s="41"/>
       <c r="N40" s="41"/>
@@ -4961,7 +4961,7 @@
         <v>14</v>
       </c>
       <c r="C42" s="29">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
@@ -4989,7 +4989,7 @@
         <v>15</v>
       </c>
       <c r="C43" s="29">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
@@ -5019,7 +5019,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="28">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -5034,7 +5034,7 @@
         <v>46</v>
       </c>
       <c r="L44" s="28">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
@@ -5049,7 +5049,7 @@
         <v>17</v>
       </c>
       <c r="C45" s="40">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="D45" s="41"/>
       <c r="E45" s="41"/>
@@ -5062,7 +5062,7 @@
         <v>47</v>
       </c>
       <c r="L45" s="40">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="M45" s="41"/>
       <c r="N45" s="41"/>
@@ -5087,9 +5087,7 @@
       <c r="K46" s="43">
         <v>48</v>
       </c>
-      <c r="L46" s="29">
-        <v>130</v>
-      </c>
+      <c r="L46" s="29"/>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17"/>
@@ -5103,7 +5101,7 @@
         <v>19</v>
       </c>
       <c r="C47" s="29">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -5116,7 +5114,7 @@
         <v>49</v>
       </c>
       <c r="L47" s="29">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -5131,7 +5129,7 @@
         <v>20</v>
       </c>
       <c r="C48" s="29">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D48" s="17"/>
       <c r="E48" s="17"/>
@@ -5144,7 +5142,7 @@
         <v>50</v>
       </c>
       <c r="L48" s="29">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M48" s="17"/>
       <c r="N48" s="17"/>
@@ -5161,7 +5159,7 @@
         <v>21</v>
       </c>
       <c r="C49" s="28">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
@@ -5176,7 +5174,7 @@
         <v>51</v>
       </c>
       <c r="L49" s="28">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="M49" s="12"/>
       <c r="N49" s="12"/>
@@ -5191,7 +5189,7 @@
         <v>22</v>
       </c>
       <c r="C50" s="29">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
@@ -5204,7 +5202,7 @@
         <v>52</v>
       </c>
       <c r="L50" s="29">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -5243,7 +5241,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="29">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D52" s="17"/>
       <c r="E52" s="17"/>
@@ -5256,7 +5254,7 @@
         <v>54</v>
       </c>
       <c r="L52" s="29">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="M52" s="17"/>
       <c r="N52" s="17"/>
@@ -5271,7 +5269,7 @@
         <v>25</v>
       </c>
       <c r="C53" s="29">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D53" s="17"/>
       <c r="E53" s="17"/>
@@ -5284,7 +5282,7 @@
         <v>55</v>
       </c>
       <c r="L53" s="29">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M53" s="17"/>
       <c r="N53" s="17"/>
@@ -5301,7 +5299,7 @@
         <v>26</v>
       </c>
       <c r="C54" s="28">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -5316,7 +5314,7 @@
         <v>56</v>
       </c>
       <c r="L54" s="28">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M54" s="12"/>
       <c r="N54" s="12"/>
@@ -5344,7 +5342,7 @@
         <v>57</v>
       </c>
       <c r="L55" s="29">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="M55" s="17"/>
       <c r="N55" s="17"/>
@@ -5383,7 +5381,7 @@
         <v>29</v>
       </c>
       <c r="C57" s="29">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
@@ -5396,7 +5394,7 @@
         <v>59</v>
       </c>
       <c r="L57" s="29">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="M57" s="17"/>
       <c r="N57" s="17"/>
@@ -5424,7 +5422,7 @@
         <v>60</v>
       </c>
       <c r="L58" s="31">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="M58" s="25"/>
       <c r="N58" s="25"/>
@@ -5540,7 +5538,7 @@
         <v>25</v>
       </c>
       <c r="L2" s="28">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -5568,7 +5566,7 @@
         <v>26</v>
       </c>
       <c r="L3" s="29">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
@@ -5596,7 +5594,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="29">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
@@ -5624,7 +5622,7 @@
         <v>28</v>
       </c>
       <c r="L5" s="46">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M5" s="20"/>
       <c r="N5" s="20"/>
@@ -5667,7 +5665,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="29">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
@@ -5680,7 +5678,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="29">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
@@ -5723,7 +5721,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="29">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
@@ -5736,7 +5734,7 @@
         <v>32</v>
       </c>
       <c r="L9" s="29">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
@@ -5753,7 +5751,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="28">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
@@ -5768,7 +5766,7 @@
         <v>33</v>
       </c>
       <c r="L10" s="28">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -5783,7 +5781,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="29">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="17"/>
@@ -5811,7 +5809,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="29">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -5824,7 +5822,7 @@
         <v>35</v>
       </c>
       <c r="L12" s="29">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
@@ -5839,7 +5837,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="46">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D13" s="20"/>
       <c r="E13" s="20"/>
@@ -5852,7 +5850,7 @@
         <v>36</v>
       </c>
       <c r="L13" s="46">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="M13" s="20"/>
       <c r="N13" s="20"/>
@@ -5880,7 +5878,7 @@
         <v>37</v>
       </c>
       <c r="L14" s="29">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
@@ -5895,7 +5893,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="29">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D15" s="17"/>
       <c r="E15" s="17"/>
@@ -5908,7 +5906,7 @@
         <v>38</v>
       </c>
       <c r="L15" s="29">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
@@ -5923,7 +5921,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="29">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
@@ -5951,7 +5949,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="29">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
@@ -5964,7 +5962,7 @@
         <v>40</v>
       </c>
       <c r="L17" s="29">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
@@ -5996,7 +5994,7 @@
         <v>41</v>
       </c>
       <c r="L18" s="28">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
@@ -6095,7 +6093,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="29">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -6108,7 +6106,7 @@
         <v>45</v>
       </c>
       <c r="L22" s="29">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
@@ -6123,7 +6121,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="29">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -6136,7 +6134,7 @@
         <v>46</v>
       </c>
       <c r="L23" s="29">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
@@ -6151,7 +6149,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="29">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
@@ -6164,7 +6162,7 @@
         <v>47</v>
       </c>
       <c r="L24" s="29">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
@@ -6192,7 +6190,7 @@
         <v>48</v>
       </c>
       <c r="L25" s="31">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M25" s="25"/>
       <c r="N25" s="25"/>
@@ -6269,7 +6267,7 @@
         <v>49</v>
       </c>
       <c r="C29" s="28">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -6284,7 +6282,7 @@
         <v>73</v>
       </c>
       <c r="L29" s="28">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
@@ -6299,7 +6297,7 @@
         <v>50</v>
       </c>
       <c r="C30" s="29">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D30" s="17"/>
       <c r="E30" s="17"/>
@@ -6312,7 +6310,7 @@
         <v>74</v>
       </c>
       <c r="L30" s="29">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
@@ -6327,7 +6325,7 @@
         <v>51</v>
       </c>
       <c r="C31" s="29">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -6340,7 +6338,7 @@
         <v>75</v>
       </c>
       <c r="L31" s="29">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
@@ -6355,7 +6353,7 @@
         <v>52</v>
       </c>
       <c r="C32" s="29">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
@@ -6368,7 +6366,7 @@
         <v>76</v>
       </c>
       <c r="L32" s="46">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="M32" s="20"/>
       <c r="N32" s="20"/>
@@ -6383,7 +6381,7 @@
         <v>53</v>
       </c>
       <c r="C33" s="29">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D33" s="17"/>
       <c r="E33" s="17"/>
@@ -6396,7 +6394,7 @@
         <v>77</v>
       </c>
       <c r="L33" s="29">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
@@ -6411,7 +6409,7 @@
         <v>54</v>
       </c>
       <c r="C34" s="29">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D34" s="17"/>
       <c r="E34" s="17"/>
@@ -6424,7 +6422,7 @@
         <v>78</v>
       </c>
       <c r="L34" s="29">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
@@ -6439,7 +6437,7 @@
         <v>55</v>
       </c>
       <c r="C35" s="29">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D35" s="17"/>
       <c r="E35" s="17"/>
@@ -6452,7 +6450,7 @@
         <v>79</v>
       </c>
       <c r="L35" s="29">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
@@ -6467,7 +6465,7 @@
         <v>56</v>
       </c>
       <c r="C36" s="29">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D36" s="17"/>
       <c r="E36" s="17"/>
@@ -6480,7 +6478,7 @@
         <v>80</v>
       </c>
       <c r="L36" s="29">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
@@ -6497,7 +6495,7 @@
         <v>57</v>
       </c>
       <c r="C37" s="28">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
@@ -6512,7 +6510,7 @@
         <v>81</v>
       </c>
       <c r="L37" s="28">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M37" s="12"/>
       <c r="N37" s="12"/>
@@ -6527,7 +6525,7 @@
         <v>58</v>
       </c>
       <c r="C38" s="29">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -6540,7 +6538,7 @@
         <v>82</v>
       </c>
       <c r="L38" s="29">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
@@ -6555,7 +6553,7 @@
         <v>59</v>
       </c>
       <c r="C39" s="29">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
@@ -6568,7 +6566,7 @@
         <v>83</v>
       </c>
       <c r="L39" s="29">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
@@ -6596,7 +6594,7 @@
         <v>84</v>
       </c>
       <c r="L40" s="46">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="M40" s="20"/>
       <c r="N40" s="20"/>
@@ -6611,7 +6609,7 @@
         <v>61</v>
       </c>
       <c r="C41" s="29">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
@@ -6639,7 +6637,7 @@
         <v>62</v>
       </c>
       <c r="C42" s="29">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
@@ -6652,7 +6650,7 @@
         <v>86</v>
       </c>
       <c r="L42" s="29">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
@@ -6667,7 +6665,7 @@
         <v>63</v>
       </c>
       <c r="C43" s="29">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
@@ -6680,7 +6678,7 @@
         <v>87</v>
       </c>
       <c r="L43" s="29">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
@@ -6695,7 +6693,7 @@
         <v>64</v>
       </c>
       <c r="C44" s="29">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
@@ -6708,7 +6706,7 @@
         <v>88</v>
       </c>
       <c r="L44" s="29">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
@@ -6725,7 +6723,7 @@
         <v>65</v>
       </c>
       <c r="C45" s="28">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D45" s="12"/>
       <c r="E45" s="12"/>
@@ -6755,7 +6753,7 @@
         <v>66</v>
       </c>
       <c r="C46" s="29">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
@@ -6768,7 +6766,7 @@
         <v>90</v>
       </c>
       <c r="L46" s="29">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
@@ -6783,7 +6781,7 @@
         <v>67</v>
       </c>
       <c r="C47" s="29">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D47" s="17"/>
       <c r="E47" s="17"/>
@@ -6796,7 +6794,7 @@
         <v>91</v>
       </c>
       <c r="L47" s="29">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M47" s="17"/>
       <c r="N47" s="17"/>
@@ -6811,7 +6809,7 @@
         <v>68</v>
       </c>
       <c r="C48" s="46">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D48" s="20"/>
       <c r="E48" s="20"/>
@@ -6824,7 +6822,7 @@
         <v>92</v>
       </c>
       <c r="L48" s="46">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="M48" s="20"/>
       <c r="N48" s="20"/>
@@ -6839,7 +6837,7 @@
         <v>69</v>
       </c>
       <c r="C49" s="29">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D49" s="17"/>
       <c r="E49" s="17"/>
@@ -6852,7 +6850,7 @@
         <v>93</v>
       </c>
       <c r="L49" s="29">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="M49" s="17"/>
       <c r="N49" s="17"/>
@@ -6867,7 +6865,7 @@
         <v>70</v>
       </c>
       <c r="C50" s="29">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D50" s="17"/>
       <c r="E50" s="17"/>
@@ -6880,7 +6878,7 @@
         <v>94</v>
       </c>
       <c r="L50" s="29">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="M50" s="17"/>
       <c r="N50" s="17"/>
@@ -6908,7 +6906,7 @@
         <v>95</v>
       </c>
       <c r="L51" s="29">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="M51" s="17"/>
       <c r="N51" s="17"/>
@@ -6936,7 +6934,7 @@
         <v>96</v>
       </c>
       <c r="L52" s="31">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="M52" s="25"/>
       <c r="N52" s="25"/>

</xml_diff>